<commit_message>
rename "mount" to "quantity"
</commit_message>
<xml_diff>
--- a/resources/views/document_torg12.xlsx
+++ b/resources/views/document_torg12.xlsx
@@ -197,7 +197,7 @@
     <t xml:space="preserve">{{ items.mountPlaces }}</t>
   </si>
   <si>
-    <t xml:space="preserve">{{ items.mount }}</t>
+    <t xml:space="preserve">{{ items.quantity }}</t>
   </si>
   <si>
     <t xml:space="preserve">{{ items.price }}</t>
@@ -932,7 +932,7 @@
   <dimension ref="A1:AO48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
+      <selection pane="topLeft" activeCell="V24" activeCellId="0" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -951,7 +951,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="5.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="0.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="4.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="4.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="1.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="6.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="0.66"/>
@@ -959,7 +959,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="2.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="3.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="1" width="3.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="8.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="8.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="2.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="1.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="4.66"/>

</xml_diff>